<commit_message>
Update plan version 2.0
Update activities of plan. Insert activity: "Tìm hiểu Recommender Systems trong website thương mại".
</commit_message>
<xml_diff>
--- a/Plan & Task/PlanProject.xlsx
+++ b/Plan & Task/PlanProject.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>STT</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>PLAN DELAY</t>
+  </si>
+  <si>
+    <t>Tìm hiểu Recommender Systems và ứng dụng của nó trong website thương mại</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Cẩm Thu (Tổng hợp)</t>
   </si>
 </sst>
 </file>
@@ -255,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -278,11 +284,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -296,12 +339,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -326,10 +363,31 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -612,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F7" sqref="F7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -623,13 +681,13 @@
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="16" style="3" customWidth="1"/>
     <col min="3" max="3" width="45.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="20.5703125" style="1" customWidth="1"/>
@@ -637,80 +695,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="5" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -719,11 +777,11 @@
       <c r="E7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="7" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -732,408 +790,436 @@
       <c r="J7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="33" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+    <row r="8" spans="1:13" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>1</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="12">
         <v>43377</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="12">
         <v>43382</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="13">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="11">
         <f>E8-D8+1</f>
         <v>6</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>2</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="12">
+        <v>43377</v>
+      </c>
+      <c r="E9" s="12">
+        <v>43382</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="11">
+        <f>E9-D9+1</f>
+        <v>6</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="12" t="s">
+      <c r="J9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="12" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:13" ht="33" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>2</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>3</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D13" s="12">
         <v>43377</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E13" s="12">
         <v>43382</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="13">
-        <f>E12-D12+1</f>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="11">
+        <f>E13-D13+1</f>
         <v>6</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="12" t="s">
+      <c r="J13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="12" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="12" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:13" ht="33" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>3</v>
-      </c>
-      <c r="B16" s="9" t="s">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>4</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D17" s="12">
         <v>43384</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E17" s="12">
         <v>43398</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F17" s="18">
         <v>43390</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G17" s="18">
         <v>43397</v>
       </c>
-      <c r="H16" s="13">
-        <f>E16-D16+1</f>
-        <v>15</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>4</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="11">
-        <v>43384</v>
-      </c>
-      <c r="E17" s="11">
-        <v>43398</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="13">
+      <c r="H17" s="11">
         <f>E17-D17+1</f>
         <v>15</v>
       </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="I17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="7">
+        <v>5</v>
+      </c>
+      <c r="B18" s="17"/>
       <c r="C18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="12">
+        <v>43384</v>
+      </c>
+      <c r="E18" s="12">
+        <v>43398</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="11">
+        <f>E18-D18+1</f>
+        <v>15</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="1:13" ht="33" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>5</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10" t="s">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>6</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D20" s="12">
         <v>43384</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E20" s="12">
         <v>43398</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="13">
-        <f>E19-D19+1</f>
-        <v>15</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>6</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="11">
-        <v>43384</v>
-      </c>
-      <c r="E20" s="11">
-        <v>43398</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="13">
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="11">
         <f>E20-D20+1</f>
         <v>15</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>7</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="12">
+        <v>43384</v>
+      </c>
+      <c r="E21" s="12">
+        <v>43398</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="11">
+        <f>E21-D21+1</f>
+        <v>15</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J21" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>7</v>
-      </c>
-      <c r="B21" s="7" t="s">
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D22" s="12">
         <v>43399</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E22" s="12">
         <v>43406</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="13">
-        <f>E21-D21+1</f>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="11">
+        <f>E22-D22+1</f>
         <v>8</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>8</v>
-      </c>
-      <c r="B22" s="7" t="s">
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>9</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D23" s="12">
         <v>43407</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E23" s="12">
         <v>43410</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="13">
-        <f>E22-D22+1</f>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="11">
+        <f>E23-D23+1</f>
         <v>4</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-    </row>
-    <row r="25" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
     </row>
     <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D27" s="12">
         <v>43746</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="B8:B16"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="G16:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1142,13 +1228,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="16" style="2" customWidth="1"/>
@@ -1167,184 +1253,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.25"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+    </row>
     <row r="6" spans="1:13" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="17"/>
+      <c r="H6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:13" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:13" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:13" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="16.5" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="16.5" x14ac:dyDescent="0.25"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:M1"/>

</xml_diff>

<commit_message>
Add Block Diagram, Flowchart and Update Report
</commit_message>
<xml_diff>
--- a/Plan & Task/PlanProject.xlsx
+++ b/Plan & Task/PlanProject.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>STT</t>
   </si>
@@ -52,9 +52,6 @@
     <t>2: Code</t>
   </si>
   <si>
-    <t>Code thuật toán Content-based systems</t>
-  </si>
-  <si>
     <t>Code web:</t>
   </si>
   <si>
@@ -85,19 +82,61 @@
     <t>Ngày kiểm tra tiến độ</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Code thuật toán Collaborative filtering </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(*)</t>
-    </r>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>Môn: Machine Learning / Đồ án 3</t>
+  </si>
+  <si>
+    <t>Đề tài: Ứng dụng thuật toán máy học để phát triển "Recommender Systems" trong website thương mại</t>
+  </si>
+  <si>
+    <t>Người lập</t>
+  </si>
+  <si>
+    <t>Ngày lập</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Cẩm Thu</t>
+  </si>
+  <si>
+    <t>Người thực hiện chính</t>
+  </si>
+  <si>
+    <t>Collaborators</t>
+  </si>
+  <si>
+    <t>Lâm Thành Tài</t>
+  </si>
+  <si>
+    <t>Nguyễn Thái Học</t>
+  </si>
+  <si>
+    <t>Ngày kết thúc (dự kiến)</t>
+  </si>
+  <si>
+    <t>Ngày hoàn thành</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Delay (Yes/No)</t>
+  </si>
+  <si>
+    <t>PLAN DELAY</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Cẩm Thu (Tổng hợp)</t>
+  </si>
+  <si>
+    <t>Hoàn thành</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Tìm hiểu chung về thương mại điện tử</t>
   </si>
   <si>
     <r>
@@ -130,7 +169,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Content-based systems</t>
+      <t>Collaborative filtering</t>
     </r>
     <r>
       <rPr>
@@ -140,68 +179,32 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> và ứng dụng thuật toán này đến hết các giai đoạn ra sản phẩm cuối cùng. Nếu trong thời gian làm thuật toán Content-based systems còn thời gian thì nhóm sẽ quay trở lại giai đoạn 2 thực hiện tiếp thực toán còn lại.</t>
+      <t xml:space="preserve"> và ứng dụng thuật toán này đến hết các giai đoạn ra sản phẩm cuối cùng. Nếu trong thời gian làm thuật toán Collaborative filtering còn thời gian thì nhóm sẽ quay trở lại giai đoạn 2 thực hiện tiếp thực toán còn lại.</t>
     </r>
   </si>
   <si>
-    <t>PLAN</t>
-  </si>
-  <si>
-    <t>Môn: Machine Learning / Đồ án 3</t>
-  </si>
-  <si>
-    <t>Đề tài: Ứng dụng thuật toán máy học để phát triển "Recommender Systems" trong website thương mại</t>
-  </si>
-  <si>
-    <t>Người lập</t>
-  </si>
-  <si>
-    <t>Ngày lập</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Cẩm Thu</t>
-  </si>
-  <si>
-    <t>Người thực hiện chính</t>
-  </si>
-  <si>
-    <t>Collaborators</t>
-  </si>
-  <si>
-    <t>Lâm Thành Tài</t>
-  </si>
-  <si>
-    <t>Nguyễn Thái Học</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Cẩm Thu, Lâm Thành Tài</t>
-  </si>
-  <si>
-    <t>Ngày kết thúc (dự kiến)</t>
-  </si>
-  <si>
-    <t>Ngày hoàn thành</t>
-  </si>
-  <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
-    <t>Delay (Yes/No)</t>
-  </si>
-  <si>
-    <t>PLAN DELAY</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Cẩm Thu (Tổng hợp)</t>
-  </si>
-  <si>
-    <t>Hoàn thành</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Tìm hiểu chung về thương mại điện tử</t>
+    <t xml:space="preserve">Code thuật toán Collaborative filtering </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Code thuật toán Content-based systems </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <t>5: Document</t>
+  </si>
+  <si>
+    <t>Slide, Report</t>
   </si>
 </sst>
 </file>
@@ -331,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -374,6 +377,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -684,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -696,7 +705,7 @@
     <col min="4" max="4" width="15.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="2" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="2" customWidth="1"/>
@@ -707,71 +716,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="A1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="A2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
+      <c r="A3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
     </row>
     <row r="5" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="B5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -787,40 +796,40 @@
         <v>3</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="19"/>
+        <v>30</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="21"/>
       <c r="H7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>1</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D8" s="12">
         <v>43377</v>
@@ -835,26 +844,26 @@
         <v>6</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="9">
         <v>43382</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="33" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="A9" s="21">
         <v>2</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="12">
         <v>43377</v>
@@ -869,24 +878,24 @@
         <v>6</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K9" s="9">
         <v>43382</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="10" t="s">
         <v>6</v>
       </c>
@@ -902,8 +911,8 @@
       <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
@@ -919,8 +928,8 @@
       <c r="M11" s="11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="22"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="10" t="s">
         <v>8</v>
       </c>
@@ -936,12 +945,12 @@
       <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="33" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="21">
         <v>3</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="12">
         <v>43377</v>
@@ -956,24 +965,24 @@
         <v>6</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K13" s="9">
         <v>43382</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M13" s="11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="10" t="s">
         <v>6</v>
       </c>
@@ -989,8 +998,8 @@
       <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="10" t="s">
         <v>7</v>
       </c>
@@ -1006,8 +1015,8 @@
       <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="10" t="s">
         <v>8</v>
       </c>
@@ -1022,78 +1031,78 @@
       <c r="L16" s="8"/>
       <c r="M16" s="11"/>
     </row>
-    <row r="17" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>4</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D17" s="12">
         <v>43384</v>
       </c>
       <c r="E17" s="12">
-        <v>43398</v>
-      </c>
-      <c r="F17" s="20">
+        <v>43414</v>
+      </c>
+      <c r="F17" s="22">
         <v>43390</v>
       </c>
-      <c r="G17" s="20">
-        <v>43397</v>
+      <c r="G17" s="22">
+        <v>43410</v>
       </c>
       <c r="H17" s="11">
         <f>E17-D17+1</f>
-        <v>15</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="33" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="8" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D18" s="12">
         <v>43384</v>
       </c>
       <c r="E18" s="12">
-        <v>43398</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
+        <v>43414</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="11">
         <f>E18-D18+1</f>
-        <v>15</v>
-      </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="11"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="19"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -1105,27 +1114,27 @@
       <c r="A20" s="5">
         <v>6</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="12">
         <v>43384</v>
       </c>
       <c r="E20" s="12">
-        <v>43398</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
+        <v>43414</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="11">
         <f>E20-D20+1</f>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
@@ -1135,27 +1144,27 @@
       <c r="A21" s="5">
         <v>7</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="12">
         <v>43384</v>
       </c>
       <c r="E21" s="12">
-        <v>43398</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
+        <v>43414</v>
+      </c>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="11">
         <f>E21-D21+1</f>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
@@ -1166,10 +1175,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="12">
         <v>43399</v>
@@ -1194,10 +1203,10 @@
         <v>9</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="D23" s="12">
         <v>43407</v>
@@ -1217,21 +1226,51 @@
       <c r="L23" s="8"/>
       <c r="M23" s="11"/>
     </row>
+    <row r="24" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>10</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="16">
+        <v>43377</v>
+      </c>
+      <c r="E24" s="16">
+        <v>43419</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="11">
+        <f>E24-D24+1</f>
+        <v>43</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="11"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="11"/>
+    </row>
     <row r="26" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D27" s="12">
         <v>43746</v>
@@ -1261,7 +1300,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1283,55 +1322,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="A1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="A2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
+      <c r="A3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1347,29 +1386,29 @@
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="19"/>
+        <v>30</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="21"/>
       <c r="H6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>